<commit_message>
filled in in for our hypothetical randstad graph
</commit_message>
<xml_diff>
--- a/Data_files/Graph_randstad.xlsx
+++ b/Data_files/Graph_randstad.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365.sharepoint.com/sites/DesigninNetwork/Gedeelde documenten/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_6A47418DB8C39B5267FDCF3BDB64C7E63773F567" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{571AEE17-2B0C-40EC-81BF-3876B7890CD8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A416182-B034-44D8-A7E8-0FE86E3B096E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="1100" windowWidth="19170" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Cities</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Employees</t>
   </si>
   <si>
-    <t>Lattitude</t>
-  </si>
-  <si>
     <t>Longitude</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Delft</t>
   </si>
   <si>
-    <t>Den Haag </t>
-  </si>
-  <si>
     <t>Dordrecht</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>Rotterdam</t>
   </si>
   <si>
-    <t>Schiphol, Haarlemmermeer</t>
-  </si>
-  <si>
     <t>Spijkenisse</t>
   </si>
   <si>
@@ -114,6 +105,15 @@
   </si>
   <si>
     <t>Zoetermeer</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Den Haag</t>
+  </si>
+  <si>
+    <t>Schiphol Haarlemmermeer</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,78 +484,78 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>2</v>
+      </c>
+      <c r="I1">
+        <v>3</v>
+      </c>
+      <c r="J1">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Y1">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1">
         <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>111834</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>222825</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>114182</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>160759</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>918117</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>106086</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>562839</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>121434</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>75316</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>165396</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>93345</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>127089</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>663900</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>162300</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>72561</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>367947</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>75079</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>114887</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>53244</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>159618</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>126998</v>

</xml_diff>

<commit_message>
cleanup coordinates and fixed some connections
</commit_message>
<xml_diff>
--- a/Data_files/Graph_randstad.xlsx
+++ b/Data_files/Graph_randstad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A416182-B034-44D8-A7E8-0FE86E3B096E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A692E9B-841D-47AA-8C53-9C3B51F471CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -567,7 +567,7 @@
         <v>52.631599999999999</v>
       </c>
       <c r="E2">
-        <v>4.7487000000000004</v>
+        <v>4.7534000000000001</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -644,10 +644,10 @@
         <v>243.4843554</v>
       </c>
       <c r="D3">
-        <v>52.367600000000003</v>
+        <v>52.3508</v>
       </c>
       <c r="E3">
-        <v>5.2321999999999997</v>
+        <v>5.2647000000000004</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -724,10 +724,10 @@
         <v>124.7684536</v>
       </c>
       <c r="D4">
-        <v>52.129199999999997</v>
+        <v>52.111199999999997</v>
       </c>
       <c r="E4">
-        <v>4.6555</v>
+        <v>4.6473000000000004</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -964,10 +964,10 @@
         <v>115.921828</v>
       </c>
       <c r="D7">
-        <v>51.999000000000002</v>
+        <v>52.011600000000001</v>
       </c>
       <c r="E7">
-        <v>4.3628</v>
+        <v>4.3571</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1127,7 +1127,7 @@
         <v>51.813299999999998</v>
       </c>
       <c r="E9">
-        <v>4.6905000000000001</v>
+        <v>4.6901000000000002</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1204,10 +1204,10 @@
         <v>82.298968740000007</v>
       </c>
       <c r="D10">
-        <v>52.0167</v>
+        <v>52.011499999999998</v>
       </c>
       <c r="E10">
-        <v>4.7083000000000004</v>
+        <v>4.7104999999999997</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>52.3874</v>
       </c>
       <c r="E11">
-        <v>4.899</v>
+        <v>4.646299</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1444,10 +1444,10 @@
         <v>138.87213389999999</v>
       </c>
       <c r="D13">
-        <v>52.158499999999997</v>
+        <v>52.163600000000002</v>
       </c>
       <c r="E13">
-        <v>4.4930000000000003</v>
+        <v>4.4802</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1504,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="X13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13">
         <v>0</v>
@@ -1524,10 +1524,10 @@
         <v>725.45389220000004</v>
       </c>
       <c r="D14">
-        <v>51.922499999999999</v>
+        <v>51.924399999999999</v>
       </c>
       <c r="E14">
-        <v>4.4794</v>
+        <v>4.4776999999999996</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1604,10 +1604,10 @@
         <v>177.3477432</v>
       </c>
       <c r="D15">
-        <v>52.308599999999998</v>
+        <v>52.300400000000003</v>
       </c>
       <c r="E15">
-        <v>4.7638999999999996</v>
+        <v>4.6744000000000003</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1684,10 +1684,10 @@
         <v>79.288537239999997</v>
       </c>
       <c r="D16">
-        <v>51.845799999999997</v>
+        <v>51.856200000000001</v>
       </c>
       <c r="E16">
-        <v>4.3212999999999999</v>
+        <v>4.2972000000000001</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1847,7 +1847,7 @@
         <v>51.9129</v>
       </c>
       <c r="E18">
-        <v>4.3623000000000003</v>
+        <v>4.3494000000000002</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2004,10 +2004,10 @@
         <v>58.180549839999998</v>
       </c>
       <c r="D20">
-        <v>52.079099999999997</v>
+        <v>52.079799999999999</v>
       </c>
       <c r="E20">
-        <v>4.8628999999999998</v>
+        <v>4.8627000000000002</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2043,7 +2043,7 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -2084,10 +2084,10 @@
         <v>174.4170799</v>
       </c>
       <c r="D21">
-        <v>52.4405</v>
+        <v>52.442</v>
       </c>
       <c r="E21">
-        <v>4.8182999999999998</v>
+        <v>4.8292000000000002</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2164,10 +2164,10 @@
         <v>138.77269680000001</v>
       </c>
       <c r="D22">
-        <v>52.057400000000001</v>
+        <v>52.060699999999997</v>
       </c>
       <c r="E22">
-        <v>4.4936999999999996</v>
+        <v>4.4939999999999998</v>
       </c>
       <c r="F22">
         <v>0</v>

</xml_diff>

<commit_message>
added different node sizes, based on employees
</commit_message>
<xml_diff>
--- a/Data_files/Graph_randstad.xlsx
+++ b/Data_files/Graph_randstad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A692E9B-841D-47AA-8C53-9C3B51F471CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2E557B-CD37-4D63-B07C-3C06D171C67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2239,12 +2239,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2388,6 +2382,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2398,22 +2398,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245D3D22-E257-4DBB-9D53-638351F3C934}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A82C749-3C2A-47C7-ADA8-29A0588A6394}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2431,6 +2415,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245D3D22-E257-4DBB-9D53-638351F3C934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAC06B8-1F73-47DE-927D-2B7240518635}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
cleaned up the final plot
</commit_message>
<xml_diff>
--- a/Data_files/Graph_randstad.xlsx
+++ b/Data_files/Graph_randstad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2E557B-CD37-4D63-B07C-3C06D171C67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D08A09-21F5-4729-BD75-2BF198DDDB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6">
         <v>1</v>
@@ -2022,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -2239,6 +2239,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2382,12 +2388,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2398,6 +2398,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245D3D22-E257-4DBB-9D53-638351F3C934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A82C749-3C2A-47C7-ADA8-29A0588A6394}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2415,22 +2431,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245D3D22-E257-4DBB-9D53-638351F3C934}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAC06B8-1F73-47DE-927D-2B7240518635}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added the edges to a drawing of a figure
</commit_message>
<xml_diff>
--- a/Data_files/Graph_randstad.xlsx
+++ b/Data_files/Graph_randstad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D08A09-21F5-4729-BD75-2BF198DDDB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE975751-774F-42C0-B905-68A5F085303A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1175,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -1655,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -1791,7 +1791,7 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -1809,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -2239,12 +2239,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2388,6 +2382,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2398,22 +2398,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245D3D22-E257-4DBB-9D53-638351F3C934}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A82C749-3C2A-47C7-ADA8-29A0588A6394}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2431,6 +2415,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{245D3D22-E257-4DBB-9D53-638351F3C934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAC06B8-1F73-47DE-927D-2B7240518635}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
removed the simple functions that were used precisely nowhere and changed the randstad Graph_randstad.xlsx to fit better connections
</commit_message>
<xml_diff>
--- a/Data_files/Graph_randstad.xlsx
+++ b/Data_files/Graph_randstad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE975751-774F-42C0-B905-68A5F085303A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B963E1A-A275-4C02-952F-5299D8440D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,6 +33,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -468,7 +490,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,7 +594,8 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" cm="1">
+        <f t="array" ref="G2:Z2">TRANSPOSE(F3:F22)</f>
         <v>0</v>
       </c>
       <c r="H2">
@@ -655,7 +678,8 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" cm="1">
+        <f t="array" ref="H3:Z3">TRANSPOSE(G4:G22)</f>
         <v>0</v>
       </c>
       <c r="I3">
@@ -738,7 +762,8 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" cm="1">
+        <f t="array" ref="I4:Z4">TRANSPOSE(H5:H22)</f>
         <v>0</v>
       </c>
       <c r="J4">
@@ -821,7 +846,8 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5">
+      <c r="J5" cm="1">
+        <f t="array" ref="J5:Z5">TRANSPOSE(I6:I22)</f>
         <v>0</v>
       </c>
       <c r="K5">
@@ -904,7 +930,8 @@
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="K6" cm="1">
+        <f t="array" ref="K6:Z6">TRANSPOSE(J7:J22)</f>
         <v>0</v>
       </c>
       <c r="L6">
@@ -987,7 +1014,8 @@
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="L7" cm="1">
+        <f t="array" ref="L7:Z7">TRANSPOSE(K8:K22)</f>
         <v>1</v>
       </c>
       <c r="M7">
@@ -1070,7 +1098,8 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8">
+      <c r="M8" cm="1">
+        <f t="array" ref="M8:Z8">TRANSPOSE(L9:L22)</f>
         <v>0</v>
       </c>
       <c r="N8">
@@ -1153,7 +1182,8 @@
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9">
+      <c r="N9" cm="1">
+        <f t="array" ref="N9:Z9">TRANSPOSE(M10:M22)</f>
         <v>0</v>
       </c>
       <c r="O9">
@@ -1236,7 +1266,8 @@
       <c r="N10">
         <v>0</v>
       </c>
-      <c r="O10">
+      <c r="O10" cm="1">
+        <f t="array" ref="O10:Z10">TRANSPOSE(N11:N22)</f>
         <v>0</v>
       </c>
       <c r="P10">
@@ -1319,7 +1350,8 @@
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11">
+      <c r="P11" cm="1">
+        <f t="array" ref="P11:Z11">TRANSPOSE(O12:O22)</f>
         <v>0</v>
       </c>
       <c r="Q11">
@@ -1402,7 +1434,8 @@
       <c r="P12">
         <v>0</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" cm="1">
+        <f t="array" ref="Q12:Z12">TRANSPOSE(P13:P22)</f>
         <v>0</v>
       </c>
       <c r="R12">
@@ -1485,7 +1518,8 @@
       <c r="Q13">
         <v>0</v>
       </c>
-      <c r="R13">
+      <c r="R13" cm="1">
+        <f t="array" ref="R13:Z13">TRANSPOSE(Q14:Q22)</f>
         <v>0</v>
       </c>
       <c r="S13">
@@ -1568,7 +1602,8 @@
       <c r="R14">
         <v>0</v>
       </c>
-      <c r="S14">
+      <c r="S14" cm="1">
+        <f t="array" ref="S14:Z14">TRANSPOSE(R15:R22)</f>
         <v>0</v>
       </c>
       <c r="T14">
@@ -1590,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
@@ -1651,7 +1686,8 @@
       <c r="S15">
         <v>0</v>
       </c>
-      <c r="T15">
+      <c r="T15" cm="1">
+        <f t="array" ref="T15:Z15">TRANSPOSE(S16:S22)</f>
         <v>0</v>
       </c>
       <c r="U15">
@@ -1734,7 +1770,8 @@
       <c r="T16">
         <v>0</v>
       </c>
-      <c r="U16">
+      <c r="U16" cm="1">
+        <f t="array" ref="U16:Z16">TRANSPOSE(T17:T22)</f>
         <v>0</v>
       </c>
       <c r="V16">
@@ -1817,7 +1854,8 @@
       <c r="U17">
         <v>0</v>
       </c>
-      <c r="V17">
+      <c r="V17" cm="1">
+        <f t="array" ref="V17:Z17">TRANSPOSE(U18:U22)</f>
         <v>0</v>
       </c>
       <c r="W17">
@@ -1900,7 +1938,8 @@
       <c r="V18">
         <v>0</v>
       </c>
-      <c r="W18">
+      <c r="W18" cm="1">
+        <f t="array" ref="W18:Z18">TRANSPOSE(V19:V22)</f>
         <v>1</v>
       </c>
       <c r="X18">
@@ -1983,7 +2022,8 @@
       <c r="W19">
         <v>0</v>
       </c>
-      <c r="X19">
+      <c r="X19" cm="1">
+        <f t="array" ref="X19:Z19">TRANSPOSE(W20:W22)</f>
         <v>0</v>
       </c>
       <c r="Y19">
@@ -2066,7 +2106,8 @@
       <c r="X20">
         <v>0</v>
       </c>
-      <c r="Y20">
+      <c r="Y20" cm="1">
+        <f t="array" ref="Y20:Z20">TRANSPOSE(X21:X22)</f>
         <v>0</v>
       </c>
       <c r="Z20">
@@ -2149,7 +2190,8 @@
       <c r="Y21">
         <v>0</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" cm="1">
+        <f t="array" ref="Z21">TRANSPOSE(Y22)</f>
         <v>0</v>
       </c>
     </row>
@@ -2206,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="R22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22">
         <v>0</v>

</xml_diff>

<commit_message>
some minor modifications around the Delft area
</commit_message>
<xml_diff>
--- a/Data_files/Graph_randstad.xlsx
+++ b/Data_files/Graph_randstad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E8213D-C06E-4E82-8437-010F9493E500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9859D0-0802-4116-87C1-77AEF4CF6151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="W7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X7" s="1">
         <v>1</v>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="AA7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="U14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V14" s="1">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="R17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <v>1</v>
@@ -2049,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2385,7 +2385,7 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <v>1</v>

</xml_diff>